<commit_message>
:sparkles: feature/SRM-224-test Add new rows when needed on the exported product excel
</commit_message>
<xml_diff>
--- a/storage/plantilla.xlsx
+++ b/storage/plantilla.xlsx
@@ -893,7 +893,7 @@
   <dimension ref="A1:AJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X38" activeCellId="0" sqref="X38"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,9 +1097,7 @@
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
-      <c r="S4" s="22" t="n">
-        <v>100</v>
-      </c>
+      <c r="S4" s="22"/>
       <c r="T4" s="21"/>
       <c r="U4" s="21"/>
       <c r="V4" s="22" t="n">
@@ -1152,9 +1150,7 @@
       <c r="P5" s="21"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="21"/>
-      <c r="S5" s="22" t="n">
-        <v>0</v>
-      </c>
+      <c r="S5" s="22"/>
       <c r="T5" s="21"/>
       <c r="U5" s="21"/>
       <c r="V5" s="22" t="n">
@@ -1185,793 +1181,37 @@
       <c r="AI5" s="21"/>
       <c r="AJ5" s="21"/>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="n">
-        <f aca="false">A5+1</f>
-        <v>3</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="22" t="n">
-        <f aca="false">IFERROR(J6/O6,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="22"/>
-      <c r="X6" s="22" t="n">
-        <f aca="false">S6*V6</f>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="22" t="n">
-        <f aca="false">V6*T6</f>
-        <v>0</v>
-      </c>
-      <c r="Z6" s="22" t="n">
-        <f aca="false">V6*U6</f>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="21"/>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="21"/>
-      <c r="AH6" s="21"/>
-      <c r="AI6" s="21"/>
-      <c r="AJ6" s="21"/>
-    </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="n">
-        <f aca="false">A6+1</f>
-        <v>4</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" s="21"/>
-      <c r="U7" s="21"/>
-      <c r="V7" s="22" t="n">
-        <f aca="false">IFERROR(J7/O7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W7" s="22"/>
-      <c r="X7" s="22" t="n">
-        <f aca="false">S7*V7</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="22" t="n">
-        <f aca="false">V7*T7</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="22" t="n">
-        <f aca="false">V7*U7</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="21"/>
-      <c r="AB7" s="21"/>
-      <c r="AC7" s="21"/>
-      <c r="AD7" s="21"/>
-      <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
-      <c r="AG7" s="21"/>
-      <c r="AH7" s="21"/>
-      <c r="AI7" s="21"/>
-      <c r="AJ7" s="21"/>
-    </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="n">
-        <f aca="false">A7+1</f>
-        <v>5</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="21"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="21"/>
-      <c r="U8" s="21"/>
-      <c r="V8" s="22" t="n">
-        <f aca="false">IFERROR(J8/O8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22" t="n">
-        <f aca="false">S8*V8</f>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="22" t="n">
-        <f aca="false">V8*T8</f>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="22" t="n">
-        <f aca="false">V8*U8</f>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="21"/>
-      <c r="AB8" s="21"/>
-      <c r="AC8" s="21"/>
-      <c r="AD8" s="21"/>
-      <c r="AE8" s="21"/>
-      <c r="AF8" s="21"/>
-      <c r="AG8" s="21"/>
-      <c r="AH8" s="21"/>
-      <c r="AI8" s="21"/>
-      <c r="AJ8" s="21"/>
-    </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
-        <f aca="false">A8+1</f>
-        <v>6</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="21"/>
-      <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
-      <c r="V9" s="22" t="n">
-        <f aca="false">IFERROR(J9/O9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W9" s="22"/>
-      <c r="X9" s="22" t="n">
-        <f aca="false">S9*V9</f>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="22" t="n">
-        <f aca="false">V9*T9</f>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="22" t="n">
-        <f aca="false">V9*U9</f>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="21"/>
-      <c r="AB9" s="21"/>
-      <c r="AC9" s="21"/>
-      <c r="AD9" s="21"/>
-      <c r="AE9" s="21"/>
-      <c r="AF9" s="21"/>
-      <c r="AG9" s="21"/>
-      <c r="AH9" s="21"/>
-      <c r="AI9" s="21"/>
-      <c r="AJ9" s="21"/>
-    </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="n">
-        <f aca="false">A9+1</f>
-        <v>7</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="22" t="n">
-        <f aca="false">IFERROR(J10/O10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W10" s="22"/>
-      <c r="X10" s="22" t="n">
-        <f aca="false">S10*V10</f>
-        <v>0</v>
-      </c>
-      <c r="Y10" s="22" t="n">
-        <f aca="false">V10*T10</f>
-        <v>0</v>
-      </c>
-      <c r="Z10" s="22" t="n">
-        <f aca="false">V10*U10</f>
-        <v>0</v>
-      </c>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="21"/>
-      <c r="AH10" s="21"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="21"/>
-    </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="n">
-        <f aca="false">A10+1</f>
-        <v>8</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="21"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" s="21"/>
-      <c r="U11" s="21"/>
-      <c r="V11" s="22" t="n">
-        <f aca="false">IFERROR(J11/O11,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W11" s="22"/>
-      <c r="X11" s="22" t="n">
-        <f aca="false">S11*V11</f>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="22" t="n">
-        <f aca="false">V11*T11</f>
-        <v>0</v>
-      </c>
-      <c r="Z11" s="22" t="n">
-        <f aca="false">V11*U11</f>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="21"/>
-      <c r="AB11" s="21"/>
-      <c r="AC11" s="21"/>
-      <c r="AD11" s="21"/>
-      <c r="AE11" s="21"/>
-      <c r="AF11" s="21"/>
-      <c r="AG11" s="21"/>
-      <c r="AH11" s="21"/>
-      <c r="AI11" s="21"/>
-      <c r="AJ11" s="21"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="n">
-        <f aca="false">A11+1</f>
-        <v>9</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" s="21"/>
-      <c r="U12" s="21"/>
-      <c r="V12" s="22" t="n">
-        <f aca="false">IFERROR(J12/O12,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22" t="n">
-        <f aca="false">S12*V12</f>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="22" t="n">
-        <f aca="false">V12*T12</f>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="22" t="n">
-        <f aca="false">V12*U12</f>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="21"/>
-      <c r="AB12" s="21"/>
-      <c r="AC12" s="21"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="21"/>
-      <c r="AF12" s="21"/>
-      <c r="AG12" s="21"/>
-      <c r="AH12" s="21"/>
-      <c r="AI12" s="21"/>
-      <c r="AJ12" s="21"/>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="n">
-        <f aca="false">A12+1</f>
-        <v>10</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="22" t="n">
-        <f aca="false">IFERROR(J13/O13,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W13" s="22"/>
-      <c r="X13" s="22" t="n">
-        <f aca="false">S13*V13</f>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="22" t="n">
-        <f aca="false">V13*T13</f>
-        <v>0</v>
-      </c>
-      <c r="Z13" s="22" t="n">
-        <f aca="false">V13*U13</f>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="21"/>
-      <c r="AC13" s="21"/>
-      <c r="AD13" s="21"/>
-      <c r="AE13" s="21"/>
-      <c r="AF13" s="21"/>
-      <c r="AG13" s="21"/>
-      <c r="AH13" s="21"/>
-      <c r="AI13" s="21"/>
-      <c r="AJ13" s="21"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="n">
-        <f aca="false">A13+1</f>
-        <v>11</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="22" t="n">
-        <f aca="false">IFERROR(J14/O14,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W14" s="22"/>
-      <c r="X14" s="22" t="n">
-        <f aca="false">S14*V14</f>
-        <v>0</v>
-      </c>
-      <c r="Y14" s="22" t="n">
-        <f aca="false">V14*T14</f>
-        <v>0</v>
-      </c>
-      <c r="Z14" s="22" t="n">
-        <f aca="false">V14*U14</f>
-        <v>0</v>
-      </c>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="21"/>
-      <c r="AF14" s="21"/>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="21"/>
-      <c r="AI14" s="21"/>
-      <c r="AJ14" s="21"/>
-    </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="n">
-        <f aca="false">A14+1</f>
-        <v>12</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="22" t="n">
-        <f aca="false">IFERROR(J15/O15,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22" t="n">
-        <f aca="false">S15*V15</f>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="22" t="n">
-        <f aca="false">V15*T15</f>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="22" t="n">
-        <f aca="false">V15*U15</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="21"/>
-      <c r="AI15" s="21"/>
-      <c r="AJ15" s="21"/>
-    </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="n">
-        <f aca="false">A15+1</f>
-        <v>13</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="21"/>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="21"/>
-      <c r="S16" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" s="21"/>
-      <c r="U16" s="21"/>
-      <c r="V16" s="22" t="n">
-        <f aca="false">IFERROR(J16/O16,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W16" s="22"/>
-      <c r="X16" s="22" t="n">
-        <f aca="false">S16*V16</f>
-        <v>0</v>
-      </c>
-      <c r="Y16" s="22" t="n">
-        <f aca="false">V16*T16</f>
-        <v>0</v>
-      </c>
-      <c r="Z16" s="22" t="n">
-        <f aca="false">V16*U16</f>
-        <v>0</v>
-      </c>
-      <c r="AA16" s="21"/>
-      <c r="AB16" s="21"/>
-      <c r="AC16" s="21"/>
-      <c r="AD16" s="21"/>
-      <c r="AE16" s="21"/>
-      <c r="AF16" s="21"/>
-      <c r="AG16" s="21"/>
-      <c r="AH16" s="21"/>
-      <c r="AI16" s="21"/>
-      <c r="AJ16" s="21"/>
-    </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="n">
-        <f aca="false">A16+1</f>
-        <v>14</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
-      <c r="S17" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" s="21"/>
-      <c r="U17" s="21"/>
-      <c r="V17" s="22" t="n">
-        <f aca="false">IFERROR(J17/O17,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W17" s="22"/>
-      <c r="X17" s="22" t="n">
-        <f aca="false">S17*V17</f>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="22" t="n">
-        <f aca="false">V17*T17</f>
-        <v>0</v>
-      </c>
-      <c r="Z17" s="22" t="n">
-        <f aca="false">V17*U17</f>
-        <v>0</v>
-      </c>
-      <c r="AA17" s="21"/>
-      <c r="AB17" s="21"/>
-      <c r="AC17" s="21"/>
-      <c r="AD17" s="21"/>
-      <c r="AE17" s="21"/>
-      <c r="AF17" s="21"/>
-      <c r="AG17" s="21"/>
-      <c r="AH17" s="21"/>
-      <c r="AI17" s="21"/>
-      <c r="AJ17" s="21"/>
-    </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="n">
-        <f aca="false">A17+1</f>
-        <v>15</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" s="21"/>
-      <c r="U18" s="21"/>
-      <c r="V18" s="22" t="n">
-        <f aca="false">IFERROR(J18/O18,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W18" s="22"/>
-      <c r="X18" s="22" t="n">
-        <f aca="false">S18*V18</f>
-        <v>0</v>
-      </c>
-      <c r="Y18" s="22" t="n">
-        <f aca="false">V18*T18</f>
-        <v>0</v>
-      </c>
-      <c r="Z18" s="22" t="n">
-        <f aca="false">V18*U18</f>
-        <v>0</v>
-      </c>
-      <c r="AA18" s="21"/>
-      <c r="AB18" s="21"/>
-      <c r="AC18" s="21"/>
-      <c r="AD18" s="21"/>
-      <c r="AE18" s="21"/>
-      <c r="AF18" s="21"/>
-      <c r="AG18" s="21"/>
-      <c r="AH18" s="21"/>
-      <c r="AI18" s="21"/>
-      <c r="AJ18" s="21"/>
-    </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="n">
-        <f aca="false">A18+1</f>
-        <v>16</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="22" t="n">
-        <f aca="false">IFERROR(J19/O19,0)</f>
-        <v>0</v>
-      </c>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22" t="n">
-        <f aca="false">S19*V19</f>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="22" t="n">
-        <f aca="false">V19*T19</f>
-        <v>0</v>
-      </c>
-      <c r="Z19" s="22" t="n">
-        <f aca="false">V19*U19</f>
-        <v>0</v>
-      </c>
-      <c r="AA19" s="21"/>
-      <c r="AB19" s="21"/>
-      <c r="AC19" s="21"/>
-      <c r="AD19" s="21"/>
-      <c r="AE19" s="21"/>
-      <c r="AF19" s="21"/>
-      <c r="AG19" s="21"/>
-      <c r="AH19" s="21"/>
-      <c r="AI19" s="21"/>
-      <c r="AJ19" s="21"/>
-    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -10481,20 +9721,20 @@
     <row r="8543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1046558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -12499,20 +11739,20 @@
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="33">
     <mergeCell ref="C1:D1"/>

</xml_diff>